<commit_message>
HW rev. 1 specified BOM, ERC & DRC check out, generated gerbers
</commit_message>
<xml_diff>
--- a/eagle design/cos/Čos - 5V0 converter - BOM.xlsx
+++ b/eagle design/cos/Čos - 5V0 converter - BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Čos - 5V0 converter - BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Qty</t>
   </si>
@@ -40,24 +40,15 @@
     <t>C8</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>R-EU_R0402</t>
   </si>
   <si>
     <t>R0402</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>C-EUC0603</t>
   </si>
   <si>
@@ -116,13 +107,58 @@
   </si>
   <si>
     <t>mouser url</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-TPS630701RNMR </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Texas-Instruments/TPS630701RNMR?qs=LuYMPh7GGMTyE4ON9PhzXw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-XFL4020-152MEC </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Coilcraft/XFL4020-152MEC?qs=%2Fha2pyFaduigLhcKZCbSe9QbArGlvPlxXOCFjm%2FaTBqm0TUkZLvsng%3D%3D</t>
+  </si>
+  <si>
+    <t>80-C0805C226M8</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/KEMET/C0805C226M8PACTU?qs=cGEy3R83DS93ZizaMBlKFQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0805C106M3PACLR </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/KEMET/C0805C106M3PAC7210?qs=sSYV1F9c5cFaojLA0ITCpw%3D%3D</t>
+  </si>
+  <si>
+    <t>81-GRM188R61E106MA3J</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Murata-Electronics/GRM188R61E106MA73J?qs=hNud%2FORuBR2%252B%252BY67hhW1nA%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0402C104K3P </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/KEMET/C0402C104K3PACTU?qs=gt1LBUVyoHnkmt1KfrmtmQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0402JR-7W10KL </t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Yageo/RC0402JR-7W10KL?qs=sGAEpiMZZMvdGkrng054t3bQBroXiaAZcfok9fjjif4OfQngMUmcIg%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +320,14 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -583,7 +627,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -626,12 +670,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -665,6 +714,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -965,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,7 +1029,7 @@
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="108" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -999,10 +1049,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1010,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1020,40 +1070,58 @@
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1061,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1071,40 +1139,58 @@
       </c>
       <c r="E5" t="s">
         <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1112,37 +1198,35 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="G6" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="G3" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-corrected position in BOM
</commit_message>
<xml_diff>
--- a/eagle design/cos/Čos - 5V0 converter - BOM.xlsx
+++ b/eagle design/cos/Čos - 5V0 converter - BOM.xlsx
@@ -124,9 +124,6 @@
     <t>https://hr.mouser.com/ProductDetail/Coilcraft/XFL4020-152MEC?qs=%2Fha2pyFaduigLhcKZCbSe9QbArGlvPlxXOCFjm%2FaTBqm0TUkZLvsng%3D%3D</t>
   </si>
   <si>
-    <t>80-C0805C226M8</t>
-  </si>
-  <si>
     <t>https://hr.mouser.com/ProductDetail/KEMET/C0805C226M8PACTU?qs=cGEy3R83DS93ZizaMBlKFQ%3D%3D</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Yageo/RC0402JR-7W10KL?qs=sGAEpiMZZMvdGkrng054t3bQBroXiaAZcfok9fjjif4OfQngMUmcIg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0805C226M8P </t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1072,10 +1072,10 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1095,10 +1095,10 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1118,10 +1118,10 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1141,10 +1141,10 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1164,10 +1164,10 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7">

</xml_diff>